<commit_message>
update web-06 on js automation
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/web-06.data.xlsx
+++ b/artifact/data/web-06.data.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10904"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9713E2C-3258-9B44-AD6B-3DDB5959648F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52677D69-CDEF-E847-9E21-85F65A1D366E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="19340" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="38780" windowHeight="10520" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
-    <sheet name="level1" sheetId="3" r:id="rId2"/>
+    <sheet name="xss-games" sheetId="3" r:id="rId2"/>
+    <sheet name="js1" sheetId="4" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="base">'[1]#system'!$B$2:$B$24</definedName>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="100">
   <si>
     <t>true</t>
   </si>
@@ -269,13 +270,192 @@
   </si>
   <si>
     <t>https://xss-game.appspot.com/level6/frame#data:text/javascript,alert('Hello')</t>
+  </si>
+  <si>
+    <t>https://www.cnn.com/</t>
+  </si>
+  <si>
+    <t>remove outbrain</t>
+  </si>
+  <si>
+    <t>var elem = document.querySelector('section.zn--idx-6'); 
+elem.parentNode.removeChild(elem);</t>
+  </si>
+  <si>
+    <t>remove partner content</t>
+  </si>
+  <si>
+    <t>var elem = document.querySelector('section.zn--idx-10'); 
+elem.parentNode.removeChild(elem);</t>
+  </si>
+  <si>
+    <t>remove video content</t>
+  </si>
+  <si>
+    <t>var elem = document.querySelector('section.zn--idx-5'); 
+elem.parentNode.removeChild(elem);</t>
+  </si>
+  <si>
+    <t>remove More CNN</t>
+  </si>
+  <si>
+    <t>var elem = document.querySelector('section.zn--idx-7'); 
+elem.parentNode.removeChild(elem);</t>
+  </si>
+  <si>
+    <t>remove CNN Photos</t>
+  </si>
+  <si>
+    <t>var elem = document.querySelector('section.zn--idx-8'); 
+elem.parentNode.removeChild(elem);</t>
+  </si>
+  <si>
+    <t>add new headlines</t>
+  </si>
+  <si>
+    <t>1st headline</t>
+  </si>
+  <si>
+    <t>haha msg</t>
+  </si>
+  <si>
+    <t>nexial title</t>
+  </si>
+  <si>
+    <t>'ul.cn--idx-2[data-vr-zone="home-top-col3"] li:nth-of-type(1)'</t>
+  </si>
+  <si>
+    <t>You have been hacked!  ;-)</t>
+  </si>
+  <si>
+    <t>https://nexiality.github.io/</t>
+  </si>
+  <si>
+    <t>nexial url</t>
+  </si>
+  <si>
+    <t>Nexial is AWESOME!</t>
+  </si>
+  <si>
+    <t>haha style</t>
+  </si>
+  <si>
+    <t>font-size:14pt; font-weight:bold; color:#f55; padding:3px 0; cursor: pointer;</t>
+  </si>
+  <si>
+    <r>
+      <t>jQuery(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>${1st headline}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>).prepend('&lt;li id="haha" onclick="alert(\'</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>${haha msg}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>\'); document.location=\'</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>${nexial url}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>\';" style="</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>${haha style}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>${nexial title}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>&lt;/li&gt;')</t>
+    </r>
+  </si>
+  <si>
+    <t>nexial.browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>remove superheader</t>
+  </si>
+  <si>
+    <t>var elem = document.querySelector('#jpampsuperheader'); 
+elem.parentNode.removeChild(elem);</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -324,6 +504,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="5" tint="-0.499984740745262"/>
       <name val="Courier New"/>
       <family val="1"/>
     </font>
@@ -384,7 +571,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -412,6 +599,14 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -422,7 +617,165 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="39">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1068,7 +1421,7 @@
   <dimension ref="A1:AAA9"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -1167,21 +1520,21 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="26" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="38" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="25" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="37" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="24" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="36" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="23" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="22" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="34" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1194,9 +1547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02992098-561F-1944-A340-34CB95735B3B}">
   <dimension ref="A1:AAA34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="118" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
-    </sheetView>
+    <sheetView zoomScale="112" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
@@ -1504,52 +1855,277 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A2:A23 A28:A1048576">
-    <cfRule type="beginsWith" dxfId="21" priority="18" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="33" priority="18" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A2,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="20" priority="19" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="32" priority="19" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A2,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="19" priority="20" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="20" stopIfTrue="1">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B23 B28:B1048576">
-    <cfRule type="expression" dxfId="18" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="21" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="17" priority="22">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="22">
       <formula>LEN(TRIM(B8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B7">
-    <cfRule type="expression" dxfId="16" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="16" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="15" priority="17">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="17">
       <formula>LEN(TRIM(B3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24:A27">
-    <cfRule type="beginsWith" dxfId="14" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="26" priority="11" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A24,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="13" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
+    <cfRule type="beginsWith" dxfId="25" priority="12" stopIfTrue="1" operator="beginsWith" text="nexial.">
       <formula>LEFT(A24,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="12" priority="13" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="13" stopIfTrue="1">
       <formula>LEN(TRIM(A24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:B27">
-    <cfRule type="expression" dxfId="11" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="14" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="10" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="15">
       <formula>LEN(TRIM(B24))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
+    <cfRule type="beginsWith" dxfId="21" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="20" priority="2" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="19" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1">
+    <cfRule type="expression" dxfId="18" priority="4" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="17" priority="5">
+      <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E3D70D-EC3E-C447-9A0C-FB9A745CCD4A}">
+  <dimension ref="A1:AAA14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="112" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="21.1640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="96" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:703">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="HA1" s="6"/>
+      <c r="AAA1" s="6"/>
+    </row>
+    <row r="2" spans="1:703" ht="36">
+      <c r="A2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="HA2" s="6"/>
+      <c r="AAA2" s="6"/>
+    </row>
+    <row r="3" spans="1:703" ht="36">
+      <c r="A3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="HA3" s="6"/>
+      <c r="AAA3" s="6"/>
+    </row>
+    <row r="4" spans="1:703" ht="36">
+      <c r="A4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="HA4" s="6"/>
+      <c r="AAA4" s="6"/>
+    </row>
+    <row r="5" spans="1:703" ht="36">
+      <c r="A5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="HA5" s="6"/>
+      <c r="AAA5" s="6"/>
+    </row>
+    <row r="6" spans="1:703" ht="36">
+      <c r="A6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="HA6" s="6"/>
+      <c r="AAA6" s="6"/>
+    </row>
+    <row r="7" spans="1:703" ht="36">
+      <c r="A7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="HA7" s="6"/>
+      <c r="AAA7" s="6"/>
+    </row>
+    <row r="8" spans="1:703">
+      <c r="A8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="HA8" s="6"/>
+      <c r="AAA8" s="6"/>
+    </row>
+    <row r="9" spans="1:703">
+      <c r="A9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="HA9" s="4"/>
+      <c r="AAA9" s="5"/>
+    </row>
+    <row r="10" spans="1:703">
+      <c r="A10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="HA10" s="4"/>
+      <c r="AAA10" s="5"/>
+    </row>
+    <row r="11" spans="1:703">
+      <c r="A11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="HA11" s="4"/>
+      <c r="AAA11" s="5"/>
+    </row>
+    <row r="12" spans="1:703">
+      <c r="A12" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="HA12" s="4"/>
+      <c r="AAA12" s="5"/>
+    </row>
+    <row r="13" spans="1:703">
+      <c r="A13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:703">
+      <c r="A14" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A3:A24 A29:A1048576">
+    <cfRule type="beginsWith" dxfId="16" priority="13" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A3,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="15" priority="14" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A3,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="14" priority="15" stopIfTrue="1">
+      <formula>LEN(TRIM(A3))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:B24 B29:B1048576">
+    <cfRule type="expression" dxfId="13" priority="16" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="12" priority="17">
+      <formula>LEN(TRIM(B9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:B8">
+    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="10" priority="12">
+      <formula>LEN(TRIM(B4))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25:A28">
+    <cfRule type="beginsWith" dxfId="9" priority="6" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
+      <formula>LEFT(A25,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="8" priority="7" stopIfTrue="1" operator="beginsWith" text="nexial.">
+      <formula>LEFT(A25,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8" stopIfTrue="1">
+      <formula>LEN(TRIM(A25))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25:B28">
+    <cfRule type="expression" dxfId="6" priority="9" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="5" priority="10">
+      <formula>LEN(TRIM(B25))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A2">
     <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>

</xml_diff>